<commit_message>
Jeff's Initial Setup in R
Leaving Excel and restarting in R
</commit_message>
<xml_diff>
--- a/Plate Analysis v2 5-4-15.xlsx
+++ b/Plate Analysis v2 5-4-15.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="0" windowWidth="30640" windowHeight="18840" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="880" yWindow="0" windowWidth="17720" windowHeight="8400" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="6" r:id="rId1"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="191">
   <si>
     <t>F4</t>
   </si>
@@ -688,6 +688,9 @@
   <si>
     <t>LB Water+ Replicate 3</t>
   </si>
+  <si>
+    <t>Row Number</t>
+  </si>
 </sst>
 </file>
 
@@ -784,9 +787,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="80">
+  <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -886,7 +891,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="80">
+  <cellStyles count="82">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -926,6 +931,7 @@
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -965,6 +971,7 @@
     <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1298,7 +1305,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -69670,1391 +69677,1439 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BV86"/>
+  <dimension ref="A1:BW85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:74">
-      <c r="B2" t="str">
+    <row r="1" spans="1:75">
+      <c r="C1" t="str">
         <f>Raw!$A$62</f>
         <v>OD600</v>
       </c>
     </row>
-    <row r="3" spans="1:74">
-      <c r="B3" s="5" t="str">
+    <row r="2" spans="1:75">
+      <c r="C2" s="5" t="str">
         <f>Raw!A63</f>
         <v>Cycle Nr.</v>
       </c>
-      <c r="C3" s="5">
+      <c r="D2" s="5">
         <f>Raw!B63</f>
         <v>1</v>
       </c>
-      <c r="D3" s="5">
+      <c r="E2" s="5">
         <f>Raw!C63</f>
         <v>2</v>
       </c>
-      <c r="E3" s="5">
+      <c r="F2" s="5">
         <f>Raw!D63</f>
         <v>3</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G2" s="5">
         <f>Raw!E63</f>
         <v>4</v>
       </c>
-      <c r="G3" s="5">
+      <c r="H2" s="5">
         <f>Raw!F63</f>
         <v>5</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I2" s="5">
         <f>Raw!G63</f>
         <v>6</v>
       </c>
-      <c r="I3" s="5">
+      <c r="J2" s="5">
         <f>Raw!H63</f>
         <v>7</v>
       </c>
-      <c r="J3" s="5">
+      <c r="K2" s="5">
         <f>Raw!I63</f>
         <v>8</v>
       </c>
-      <c r="K3" s="5">
+      <c r="L2" s="5">
         <f>Raw!J63</f>
         <v>9</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M2" s="5">
         <f>Raw!K63</f>
         <v>10</v>
       </c>
-      <c r="M3" s="5">
+      <c r="N2" s="5">
         <f>Raw!L63</f>
         <v>11</v>
       </c>
-      <c r="N3" s="5">
+      <c r="O2" s="5">
         <f>Raw!M63</f>
         <v>12</v>
       </c>
-      <c r="O3" s="5">
+      <c r="P2" s="5">
         <f>Raw!N63</f>
         <v>13</v>
       </c>
-      <c r="P3" s="5">
+      <c r="Q2" s="5">
         <f>Raw!O63</f>
         <v>14</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="R2" s="5">
         <f>Raw!P63</f>
         <v>15</v>
       </c>
-      <c r="R3" s="5">
+      <c r="S2" s="5">
         <f>Raw!Q63</f>
         <v>16</v>
       </c>
-      <c r="S3" s="5">
+      <c r="T2" s="5">
         <f>Raw!R63</f>
         <v>17</v>
       </c>
-      <c r="T3" s="5">
+      <c r="U2" s="5">
         <f>Raw!S63</f>
         <v>18</v>
       </c>
-      <c r="U3" s="5">
+      <c r="V2" s="5">
         <f>Raw!T63</f>
         <v>19</v>
       </c>
-      <c r="V3" s="5">
+      <c r="W2" s="5">
         <f>Raw!U63</f>
         <v>20</v>
       </c>
-      <c r="W3" s="5">
+      <c r="X2" s="5">
         <f>Raw!V63</f>
         <v>21</v>
       </c>
-      <c r="X3" s="5">
+      <c r="Y2" s="5">
         <f>Raw!W63</f>
         <v>22</v>
       </c>
-      <c r="Y3" s="5">
+      <c r="Z2" s="5">
         <f>Raw!X63</f>
         <v>23</v>
       </c>
-      <c r="Z3" s="5">
+      <c r="AA2" s="5">
         <f>Raw!Y63</f>
         <v>24</v>
       </c>
-      <c r="AA3" s="5">
+      <c r="AB2" s="5">
         <f>Raw!Z63</f>
         <v>25</v>
       </c>
-      <c r="AB3" s="5">
+      <c r="AC2" s="5">
         <f>Raw!AA63</f>
         <v>26</v>
       </c>
-      <c r="AC3" s="5">
+      <c r="AD2" s="5">
         <f>Raw!AB63</f>
         <v>27</v>
       </c>
-      <c r="AD3" s="5">
+      <c r="AE2" s="5">
         <f>Raw!AC63</f>
         <v>28</v>
       </c>
-      <c r="AE3" s="5">
+      <c r="AF2" s="5">
         <f>Raw!AD63</f>
         <v>29</v>
       </c>
-      <c r="AF3" s="5">
+      <c r="AG2" s="5">
         <f>Raw!AE63</f>
         <v>30</v>
       </c>
-      <c r="AG3" s="5">
+      <c r="AH2" s="5">
         <f>Raw!AF63</f>
         <v>31</v>
       </c>
-      <c r="AH3" s="5">
+      <c r="AI2" s="5">
         <f>Raw!AG63</f>
         <v>32</v>
       </c>
-      <c r="AI3" s="5">
+      <c r="AJ2" s="5">
         <f>Raw!AH63</f>
         <v>33</v>
       </c>
-      <c r="AJ3" s="5">
+      <c r="AK2" s="5">
         <f>Raw!AI63</f>
         <v>34</v>
       </c>
-      <c r="AK3" s="5">
+      <c r="AL2" s="5">
         <f>Raw!AJ63</f>
         <v>35</v>
       </c>
-      <c r="AL3" s="5">
+      <c r="AM2" s="5">
         <f>Raw!AK63</f>
         <v>36</v>
       </c>
-      <c r="AM3" s="5">
+      <c r="AN2" s="5">
         <f>Raw!AL63</f>
         <v>37</v>
       </c>
-      <c r="AN3" s="5">
+      <c r="AO2" s="5">
         <f>Raw!AM63</f>
         <v>38</v>
       </c>
-      <c r="AO3" s="5">
+      <c r="AP2" s="5">
         <f>Raw!AN63</f>
         <v>39</v>
       </c>
-      <c r="AP3" s="5">
+      <c r="AQ2" s="5">
         <f>Raw!AO63</f>
         <v>40</v>
       </c>
-      <c r="AQ3" s="5">
+      <c r="AR2" s="5">
         <f>Raw!AP63</f>
         <v>41</v>
       </c>
-      <c r="AR3" s="5">
+      <c r="AS2" s="5">
         <f>Raw!AQ63</f>
         <v>42</v>
       </c>
-      <c r="AS3" s="5">
+      <c r="AT2" s="5">
         <f>Raw!AR63</f>
         <v>43</v>
       </c>
-      <c r="AT3" s="5">
+      <c r="AU2" s="5">
         <f>Raw!AS63</f>
         <v>44</v>
       </c>
-      <c r="AU3" s="5">
+      <c r="AV2" s="5">
         <f>Raw!AT63</f>
         <v>45</v>
       </c>
-      <c r="AV3" s="5">
+      <c r="AW2" s="5">
         <f>Raw!AU63</f>
         <v>46</v>
       </c>
-      <c r="AW3" s="5">
+      <c r="AX2" s="5">
         <f>Raw!AV63</f>
         <v>47</v>
       </c>
-      <c r="AX3" s="5">
+      <c r="AY2" s="5">
         <f>Raw!AW63</f>
         <v>48</v>
       </c>
-      <c r="AY3" s="5">
+      <c r="AZ2" s="5">
         <f>Raw!AX63</f>
         <v>49</v>
       </c>
-      <c r="AZ3" s="5">
+      <c r="BA2" s="5">
         <f>Raw!AY63</f>
         <v>50</v>
       </c>
-      <c r="BA3" s="5">
+      <c r="BB2" s="5">
         <f>Raw!AZ63</f>
         <v>51</v>
       </c>
-      <c r="BB3" s="5">
+      <c r="BC2" s="5">
         <f>Raw!BA63</f>
         <v>52</v>
       </c>
-      <c r="BC3" s="5">
+      <c r="BD2" s="5">
         <f>Raw!BB63</f>
         <v>53</v>
       </c>
-      <c r="BD3" s="5">
+      <c r="BE2" s="5">
         <f>Raw!BC63</f>
         <v>54</v>
       </c>
-      <c r="BE3" s="5">
+      <c r="BF2" s="5">
         <f>Raw!BD63</f>
         <v>55</v>
       </c>
-      <c r="BF3" s="5">
+      <c r="BG2" s="5">
         <f>Raw!BE63</f>
         <v>56</v>
       </c>
-      <c r="BG3" s="5">
+      <c r="BH2" s="5">
         <f>Raw!BF63</f>
         <v>57</v>
       </c>
-      <c r="BH3" s="5">
+      <c r="BI2" s="5">
         <f>Raw!BG63</f>
         <v>58</v>
       </c>
-      <c r="BI3" s="5">
+      <c r="BJ2" s="5">
         <f>Raw!BH63</f>
         <v>59</v>
       </c>
-      <c r="BJ3" s="5">
+      <c r="BK2" s="5">
         <f>Raw!BI63</f>
         <v>60</v>
       </c>
-      <c r="BK3" s="5">
+      <c r="BL2" s="5">
         <f>Raw!BJ63</f>
         <v>61</v>
       </c>
-      <c r="BL3" s="5">
+      <c r="BM2" s="5">
         <f>Raw!BK63</f>
         <v>62</v>
       </c>
-      <c r="BM3" s="5">
+      <c r="BN2" s="5">
         <f>Raw!BL63</f>
         <v>63</v>
       </c>
-      <c r="BN3" s="5">
+      <c r="BO2" s="5">
         <f>Raw!BM63</f>
         <v>64</v>
       </c>
-      <c r="BO3" s="5">
+      <c r="BP2" s="5">
         <f>Raw!BN63</f>
         <v>65</v>
       </c>
-      <c r="BP3" s="5">
+      <c r="BQ2" s="5">
         <f>Raw!BO63</f>
         <v>66</v>
       </c>
-      <c r="BQ3" s="5">
+      <c r="BR2" s="5">
         <f>Raw!BP63</f>
         <v>67</v>
       </c>
-      <c r="BR3" s="5">
+      <c r="BS2" s="5">
         <f>Raw!BQ63</f>
         <v>68</v>
       </c>
-      <c r="BS3" s="5">
+      <c r="BT2" s="5">
         <f>Raw!BR63</f>
         <v>69</v>
       </c>
-      <c r="BT3" s="5">
+      <c r="BU2" s="5">
         <f>Raw!BS63</f>
         <v>70</v>
       </c>
-      <c r="BU3" s="5">
+      <c r="BV2" s="5">
         <f>Raw!BT63</f>
         <v>71</v>
       </c>
-      <c r="BV3" s="5">
+      <c r="BW2" s="5">
         <f>Raw!BU63</f>
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:74">
-      <c r="B4" s="5" t="str">
+    <row r="3" spans="1:75">
+      <c r="C3" s="5" t="str">
         <f>Raw!A64</f>
         <v>Time [s]</v>
       </c>
-      <c r="C4">
+      <c r="D3">
         <f>Raw!B64</f>
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="E3">
         <f>Raw!C64</f>
         <v>719.6</v>
       </c>
-      <c r="E4">
+      <c r="F3">
         <f>Raw!D64</f>
         <v>1438.5</v>
       </c>
-      <c r="F4">
+      <c r="G3">
         <f>Raw!E64</f>
         <v>2157.5</v>
       </c>
-      <c r="G4">
+      <c r="H3">
         <f>Raw!F64</f>
         <v>2876.5</v>
       </c>
-      <c r="H4">
+      <c r="I3">
         <f>Raw!G64</f>
         <v>3595.5</v>
       </c>
-      <c r="I4">
+      <c r="J3">
         <f>Raw!H64</f>
         <v>4314.5</v>
       </c>
-      <c r="J4">
+      <c r="K3">
         <f>Raw!I64</f>
         <v>5033.5</v>
       </c>
-      <c r="K4">
+      <c r="L3">
         <f>Raw!J64</f>
         <v>5752.5</v>
       </c>
-      <c r="L4">
+      <c r="M3">
         <f>Raw!K64</f>
         <v>6471.5</v>
       </c>
-      <c r="M4">
+      <c r="N3">
         <f>Raw!L64</f>
         <v>7190.5</v>
       </c>
-      <c r="N4">
+      <c r="O3">
         <f>Raw!M64</f>
         <v>7909.4</v>
       </c>
-      <c r="O4">
+      <c r="P3">
         <f>Raw!N64</f>
         <v>8628.4</v>
       </c>
-      <c r="P4">
+      <c r="Q3">
         <f>Raw!O64</f>
         <v>9347.4</v>
       </c>
-      <c r="Q4">
+      <c r="R3">
         <f>Raw!P64</f>
         <v>10066.4</v>
       </c>
-      <c r="R4">
+      <c r="S3">
         <f>Raw!Q64</f>
         <v>10785.4</v>
       </c>
-      <c r="S4">
+      <c r="T3">
         <f>Raw!R64</f>
         <v>11504.4</v>
       </c>
-      <c r="T4">
+      <c r="U3">
         <f>Raw!S64</f>
         <v>12223.4</v>
       </c>
-      <c r="U4">
+      <c r="V3">
         <f>Raw!T64</f>
         <v>12942.4</v>
       </c>
-      <c r="V4">
+      <c r="W3">
         <f>Raw!U64</f>
         <v>13661.4</v>
       </c>
-      <c r="W4">
+      <c r="X3">
         <f>Raw!V64</f>
         <v>14380.4</v>
       </c>
-      <c r="X4">
+      <c r="Y3">
         <f>Raw!W64</f>
         <v>15099.3</v>
       </c>
-      <c r="Y4">
+      <c r="Z3">
         <f>Raw!X64</f>
         <v>15818.3</v>
       </c>
-      <c r="Z4">
+      <c r="AA3">
         <f>Raw!Y64</f>
         <v>16537.3</v>
       </c>
-      <c r="AA4">
+      <c r="AB3">
         <f>Raw!Z64</f>
         <v>17256.3</v>
       </c>
-      <c r="AB4">
+      <c r="AC3">
         <f>Raw!AA64</f>
         <v>17975.3</v>
       </c>
-      <c r="AC4">
+      <c r="AD3">
         <f>Raw!AB64</f>
         <v>18694.3</v>
       </c>
-      <c r="AD4">
+      <c r="AE3">
         <f>Raw!AC64</f>
         <v>19413.400000000001</v>
       </c>
-      <c r="AE4">
+      <c r="AF3">
         <f>Raw!AD64</f>
         <v>20132.3</v>
       </c>
-      <c r="AF4">
+      <c r="AG3">
         <f>Raw!AE64</f>
         <v>20851.3</v>
       </c>
-      <c r="AG4">
+      <c r="AH3">
         <f>Raw!AF64</f>
         <v>21570.3</v>
       </c>
-      <c r="AH4">
+      <c r="AI3">
         <f>Raw!AG64</f>
         <v>22289.200000000001</v>
       </c>
-      <c r="AI4">
+      <c r="AJ3">
         <f>Raw!AH64</f>
         <v>23008.2</v>
       </c>
-      <c r="AJ4">
+      <c r="AK3">
         <f>Raw!AI64</f>
         <v>23727.200000000001</v>
       </c>
-      <c r="AK4">
+      <c r="AL3">
         <f>Raw!AJ64</f>
         <v>24446.2</v>
       </c>
-      <c r="AL4">
+      <c r="AM3">
         <f>Raw!AK64</f>
         <v>25165.200000000001</v>
       </c>
-      <c r="AM4">
+      <c r="AN3">
         <f>Raw!AL64</f>
         <v>25884.2</v>
       </c>
-      <c r="AN4">
+      <c r="AO3">
         <f>Raw!AM64</f>
         <v>26603.200000000001</v>
       </c>
-      <c r="AO4">
+      <c r="AP3">
         <f>Raw!AN64</f>
         <v>27322.2</v>
       </c>
-      <c r="AP4">
+      <c r="AQ3">
         <f>Raw!AO64</f>
         <v>28041.200000000001</v>
       </c>
-      <c r="AQ4">
+      <c r="AR3">
         <f>Raw!AP64</f>
         <v>28760.2</v>
       </c>
-      <c r="AR4">
+      <c r="AS3">
         <f>Raw!AQ64</f>
         <v>29479.1</v>
       </c>
-      <c r="AS4">
+      <c r="AT3">
         <f>Raw!AR64</f>
         <v>30198.1</v>
       </c>
-      <c r="AT4">
+      <c r="AU3">
         <f>Raw!AS64</f>
         <v>30917.1</v>
       </c>
-      <c r="AU4">
+      <c r="AV3">
         <f>Raw!AT64</f>
         <v>31636.1</v>
       </c>
-      <c r="AV4">
+      <c r="AW3">
         <f>Raw!AU64</f>
         <v>32355.1</v>
       </c>
-      <c r="AW4">
+      <c r="AX3">
         <f>Raw!AV64</f>
         <v>33074.1</v>
       </c>
-      <c r="AX4">
+      <c r="AY3">
         <f>Raw!AW64</f>
         <v>33793.1</v>
       </c>
-      <c r="AY4">
+      <c r="AZ3">
         <f>Raw!AX64</f>
         <v>34512.1</v>
       </c>
-      <c r="AZ4">
+      <c r="BA3">
         <f>Raw!AY64</f>
         <v>35231.1</v>
       </c>
-      <c r="BA4">
+      <c r="BB3">
         <f>Raw!AZ64</f>
         <v>35950.1</v>
       </c>
-      <c r="BB4">
+      <c r="BC3">
         <f>Raw!BA64</f>
         <v>36669.1</v>
       </c>
-      <c r="BC4">
+      <c r="BD3">
         <f>Raw!BB64</f>
         <v>37388</v>
       </c>
-      <c r="BD4">
+      <c r="BE3">
         <f>Raw!BC64</f>
         <v>38107</v>
       </c>
-      <c r="BE4">
+      <c r="BF3">
         <f>Raw!BD64</f>
         <v>38826</v>
       </c>
-      <c r="BF4">
+      <c r="BG3">
         <f>Raw!BE64</f>
         <v>39545</v>
       </c>
-      <c r="BG4">
+      <c r="BH3">
         <f>Raw!BF64</f>
         <v>40264</v>
       </c>
-      <c r="BH4">
+      <c r="BI3">
         <f>Raw!BG64</f>
         <v>40983</v>
       </c>
-      <c r="BI4">
+      <c r="BJ3">
         <f>Raw!BH64</f>
         <v>41702</v>
       </c>
-      <c r="BJ4">
+      <c r="BK3">
         <f>Raw!BI64</f>
         <v>42421</v>
       </c>
-      <c r="BK4">
+      <c r="BL3">
         <f>Raw!BJ64</f>
         <v>43140</v>
       </c>
-      <c r="BL4">
+      <c r="BM3">
         <f>Raw!BK64</f>
         <v>43859</v>
       </c>
-      <c r="BM4">
+      <c r="BN3">
         <f>Raw!BL64</f>
         <v>44577.9</v>
       </c>
-      <c r="BN4">
+      <c r="BO3">
         <f>Raw!BM64</f>
         <v>45296.9</v>
       </c>
-      <c r="BO4">
+      <c r="BP3">
         <f>Raw!BN64</f>
         <v>46015.9</v>
       </c>
-      <c r="BP4">
+      <c r="BQ3">
         <f>Raw!BO64</f>
         <v>46734.9</v>
       </c>
-      <c r="BQ4">
+      <c r="BR3">
         <f>Raw!BP64</f>
         <v>47453.9</v>
       </c>
-      <c r="BR4">
+      <c r="BS3">
         <f>Raw!BQ64</f>
         <v>48172.9</v>
       </c>
-      <c r="BS4">
+      <c r="BT3">
         <f>Raw!BR64</f>
         <v>48891.9</v>
       </c>
-      <c r="BT4">
+      <c r="BU3">
         <f>Raw!BS64</f>
         <v>49610.9</v>
       </c>
-      <c r="BU4">
+      <c r="BV3">
         <f>Raw!BT64</f>
         <v>50329.9</v>
       </c>
-      <c r="BV4">
+      <c r="BW3">
         <f>Raw!BU64</f>
         <v>51048.9</v>
       </c>
     </row>
-    <row r="5" spans="1:74">
-      <c r="B5" s="5" t="str">
+    <row r="4" spans="1:75">
+      <c r="B4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="5" t="str">
         <f>Raw!A65</f>
         <v>Temp. [°C]</v>
       </c>
-      <c r="C5">
+      <c r="D4">
         <f>Raw!B65</f>
         <v>37</v>
       </c>
-      <c r="D5">
+      <c r="E4">
         <f>Raw!C65</f>
         <v>36.799999999999997</v>
       </c>
-      <c r="E5">
+      <c r="F4">
         <f>Raw!D65</f>
         <v>37.1</v>
       </c>
-      <c r="F5">
+      <c r="G4">
         <f>Raw!E65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="G5">
+      <c r="H4">
         <f>Raw!F65</f>
         <v>37.1</v>
       </c>
-      <c r="H5">
+      <c r="I4">
         <f>Raw!G65</f>
         <v>36.9</v>
       </c>
-      <c r="I5">
+      <c r="J4">
         <f>Raw!H65</f>
         <v>37.1</v>
       </c>
-      <c r="J5">
+      <c r="K4">
         <f>Raw!I65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="K5">
+      <c r="L4">
         <f>Raw!J65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="L5">
+      <c r="M4">
         <f>Raw!K65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="M5">
+      <c r="N4">
         <f>Raw!L65</f>
         <v>36.799999999999997</v>
       </c>
-      <c r="N5">
+      <c r="O4">
         <f>Raw!M65</f>
         <v>37.1</v>
       </c>
-      <c r="O5">
+      <c r="P4">
         <f>Raw!N65</f>
         <v>37</v>
       </c>
-      <c r="P5">
+      <c r="Q4">
         <f>Raw!O65</f>
         <v>37.1</v>
       </c>
-      <c r="Q5">
+      <c r="R4">
         <f>Raw!P65</f>
         <v>37.1</v>
       </c>
-      <c r="R5">
+      <c r="S4">
         <f>Raw!Q65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="S5">
+      <c r="T4">
         <f>Raw!R65</f>
         <v>37.1</v>
       </c>
-      <c r="T5">
+      <c r="U4">
         <f>Raw!S65</f>
         <v>37</v>
       </c>
-      <c r="U5">
+      <c r="V4">
         <f>Raw!T65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="V5">
+      <c r="W4">
         <f>Raw!U65</f>
         <v>37.1</v>
       </c>
-      <c r="W5">
+      <c r="X4">
         <f>Raw!V65</f>
         <v>37</v>
       </c>
-      <c r="X5">
+      <c r="Y4">
         <f>Raw!W65</f>
         <v>37.299999999999997</v>
       </c>
-      <c r="Y5">
+      <c r="Z4">
         <f>Raw!X65</f>
         <v>37.299999999999997</v>
       </c>
-      <c r="Z5">
+      <c r="AA4">
         <f>Raw!Y65</f>
         <v>37.1</v>
       </c>
-      <c r="AA5">
+      <c r="AB4">
         <f>Raw!Z65</f>
         <v>37.1</v>
       </c>
-      <c r="AB5">
+      <c r="AC4">
         <f>Raw!AA65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="AC5">
+      <c r="AD4">
         <f>Raw!AB65</f>
         <v>37.1</v>
       </c>
-      <c r="AD5">
+      <c r="AE4">
         <f>Raw!AC65</f>
         <v>37.1</v>
       </c>
-      <c r="AE5">
+      <c r="AF4">
         <f>Raw!AD65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="AF5">
+      <c r="AG4">
         <f>Raw!AE65</f>
         <v>36.9</v>
       </c>
-      <c r="AG5">
+      <c r="AH4">
         <f>Raw!AF65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="AH5">
+      <c r="AI4">
         <f>Raw!AG65</f>
         <v>37.1</v>
       </c>
-      <c r="AI5">
+      <c r="AJ4">
         <f>Raw!AH65</f>
         <v>37.1</v>
       </c>
-      <c r="AJ5">
+      <c r="AK4">
         <f>Raw!AI65</f>
         <v>37</v>
       </c>
-      <c r="AK5">
+      <c r="AL4">
         <f>Raw!AJ65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="AL5">
+      <c r="AM4">
         <f>Raw!AK65</f>
         <v>37.1</v>
       </c>
-      <c r="AM5">
+      <c r="AN4">
         <f>Raw!AL65</f>
         <v>37</v>
       </c>
-      <c r="AN5">
+      <c r="AO4">
         <f>Raw!AM65</f>
         <v>37</v>
       </c>
-      <c r="AO5">
+      <c r="AP4">
         <f>Raw!AN65</f>
         <v>37.1</v>
       </c>
-      <c r="AP5">
+      <c r="AQ4">
         <f>Raw!AO65</f>
         <v>37.1</v>
       </c>
-      <c r="AQ5">
+      <c r="AR4">
         <f>Raw!AP65</f>
         <v>37.1</v>
       </c>
-      <c r="AR5">
+      <c r="AS4">
         <f>Raw!AQ65</f>
         <v>37.1</v>
       </c>
-      <c r="AS5">
+      <c r="AT4">
         <f>Raw!AR65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="AT5">
+      <c r="AU4">
         <f>Raw!AS65</f>
         <v>37.1</v>
       </c>
-      <c r="AU5">
+      <c r="AV4">
         <f>Raw!AT65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="AV5">
+      <c r="AW4">
         <f>Raw!AU65</f>
         <v>37</v>
       </c>
-      <c r="AW5">
+      <c r="AX4">
         <f>Raw!AV65</f>
         <v>36.799999999999997</v>
       </c>
-      <c r="AX5">
+      <c r="AY4">
         <f>Raw!AW65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="AY5">
+      <c r="AZ4">
         <f>Raw!AX65</f>
         <v>36.9</v>
       </c>
-      <c r="AZ5">
+      <c r="BA4">
         <f>Raw!AY65</f>
         <v>37</v>
       </c>
-      <c r="BA5">
+      <c r="BB4">
         <f>Raw!AZ65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="BB5">
+      <c r="BC4">
         <f>Raw!BA65</f>
         <v>37.1</v>
       </c>
-      <c r="BC5">
+      <c r="BD4">
         <f>Raw!BB65</f>
         <v>36.9</v>
       </c>
-      <c r="BD5">
+      <c r="BE4">
         <f>Raw!BC65</f>
         <v>37.1</v>
       </c>
-      <c r="BE5">
+      <c r="BF4">
         <f>Raw!BD65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="BF5">
+      <c r="BG4">
         <f>Raw!BE65</f>
         <v>37.299999999999997</v>
       </c>
-      <c r="BG5">
+      <c r="BH4">
         <f>Raw!BF65</f>
         <v>37.1</v>
       </c>
-      <c r="BH5">
+      <c r="BI4">
         <f>Raw!BG65</f>
         <v>37.299999999999997</v>
       </c>
-      <c r="BI5">
+      <c r="BJ4">
         <f>Raw!BH65</f>
         <v>37.1</v>
       </c>
-      <c r="BJ5">
+      <c r="BK4">
         <f>Raw!BI65</f>
         <v>37.299999999999997</v>
       </c>
-      <c r="BK5">
+      <c r="BL4">
         <f>Raw!BJ65</f>
         <v>37.1</v>
       </c>
-      <c r="BL5">
+      <c r="BM4">
         <f>Raw!BK65</f>
         <v>37.1</v>
       </c>
-      <c r="BM5">
+      <c r="BN4">
         <f>Raw!BL65</f>
         <v>37.1</v>
       </c>
-      <c r="BN5">
+      <c r="BO4">
         <f>Raw!BM65</f>
         <v>37.1</v>
       </c>
-      <c r="BO5">
+      <c r="BP4">
         <f>Raw!BN65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="BP5">
+      <c r="BQ4">
         <f>Raw!BO65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="BQ5">
+      <c r="BR4">
         <f>Raw!BP65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="BR5">
+      <c r="BS4">
         <f>Raw!BQ65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="BS5">
+      <c r="BT4">
         <f>Raw!BR65</f>
         <v>37.299999999999997</v>
       </c>
-      <c r="BT5">
+      <c r="BU4">
         <f>Raw!BS65</f>
         <v>37</v>
       </c>
-      <c r="BU5">
+      <c r="BV4">
         <f>Raw!BT65</f>
         <v>37.200000000000003</v>
       </c>
-      <c r="BV5">
+      <c r="BW4">
         <f>Raw!BU65</f>
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:74">
-      <c r="A6" t="str">
+    <row r="5" spans="1:75">
+      <c r="A5" t="str">
         <f>Setup!$A$5</f>
         <v>IodoYRS Amber+ Clone 1 IodoY+ Replicate 1</v>
       </c>
-      <c r="B6" t="str">
-        <f ca="1">INDIRECT("Raw!A"&amp;MATCH(Setup!B5,Raw!A1:A163,0))</f>
+      <c r="B5">
+        <f>MATCH(Setup!B5,Raw!$A$1:$A$163,0)</f>
+        <v>117</v>
+      </c>
+      <c r="C5" t="str">
+        <f ca="1">INDIRECT(ADDRESS(INDIRECT("B5"),1,4,TRUE,"Raw"))</f>
         <v>E4</v>
       </c>
     </row>
-    <row r="7" spans="1:74">
-      <c r="A7" t="str">
+    <row r="6" spans="1:75">
+      <c r="A6" t="str">
         <f>Setup!$A$6</f>
         <v>IodoYRS Amber+ Clone 1 IodoY+ Replicate 2</v>
       </c>
+      <c r="B6">
+        <f>MATCH(Setup!B6,Raw!$A$1:$A$163,0)</f>
+        <v>118</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ref="C6:C10" ca="1" si="0">INDIRECT("Raw!A"&amp;VALUE($B6))</f>
+        <v>E5</v>
+      </c>
     </row>
-    <row r="8" spans="1:74">
-      <c r="A8" t="str">
+    <row r="7" spans="1:75">
+      <c r="A7" t="str">
         <f>Setup!$A$7</f>
         <v>IodoYRS Amber+ Clone 1 IodoY+ Replicate 3</v>
       </c>
+      <c r="B7">
+        <f>MATCH(Setup!B7,Raw!$A$1:$A$163,0)</f>
+        <v>119</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>E6</v>
+      </c>
     </row>
-    <row r="9" spans="1:74">
-      <c r="A9" t="str">
+    <row r="8" spans="1:75">
+      <c r="A8" t="str">
         <f>Setup!$A$8</f>
         <v>IodoYRS Amber+ Clone 1 IodoY- Replicate 1</v>
       </c>
+      <c r="B8">
+        <f>MATCH(Setup!B8,Raw!$A$1:$A$163,0)</f>
+        <v>129</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F4</v>
+      </c>
     </row>
-    <row r="10" spans="1:74">
-      <c r="A10" t="str">
+    <row r="9" spans="1:75">
+      <c r="A9" t="str">
         <f>Setup!$A$9</f>
         <v>IodoYRS Amber+ Clone 1 IodoY- Replicate 2</v>
       </c>
+      <c r="B9">
+        <f>MATCH(Setup!B9,Raw!$A$1:$A$163,0)</f>
+        <v>130</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F5</v>
+      </c>
     </row>
-    <row r="11" spans="1:74">
-      <c r="A11" t="str">
+    <row r="10" spans="1:75">
+      <c r="A10" t="str">
         <f>Setup!$A$10</f>
         <v>IodoYRS Amber+ Clone 1 IodoY- Replicate 3</v>
       </c>
+      <c r="B10">
+        <f>MATCH(Setup!B10,Raw!$A$1:$A$163,0)</f>
+        <v>131</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F6</v>
+      </c>
     </row>
-    <row r="12" spans="1:74">
-      <c r="A12" t="str">
+    <row r="11" spans="1:75">
+      <c r="A11" t="str">
         <f>Setup!$D$5</f>
         <v>IodoYRS Amber+ Clone 2 IodoY+ Replicate 1</v>
       </c>
     </row>
-    <row r="13" spans="1:74">
-      <c r="A13" t="str">
+    <row r="12" spans="1:75">
+      <c r="A12" t="str">
         <f>Setup!$D$6</f>
         <v>IodoYRS Amber+ Clone 2 IodoY+ Replicate 2</v>
       </c>
     </row>
-    <row r="14" spans="1:74">
-      <c r="A14" t="str">
+    <row r="13" spans="1:75">
+      <c r="A13" t="str">
         <f>Setup!$D$7</f>
         <v>IodoYRS Amber+ Clone 2 IodoY+ Replicate 3</v>
       </c>
     </row>
-    <row r="15" spans="1:74">
-      <c r="A15" t="str">
+    <row r="14" spans="1:75">
+      <c r="A14" t="str">
         <f>Setup!$D$8</f>
         <v>IodoYRS Amber+ Clone 2 IodoY- Replicate 1</v>
       </c>
     </row>
-    <row r="16" spans="1:74">
-      <c r="A16" t="str">
+    <row r="15" spans="1:75">
+      <c r="A15" t="str">
         <f>Setup!$D$9</f>
         <v>IodoYRS Amber+ Clone 2 IodoY- Replicate 2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:75">
+      <c r="A16" t="str">
+        <f>Setup!$D$10</f>
+        <v>IodoYRS Amber+ Clone 2 IodoY- Replicate 3</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="str">
-        <f>Setup!$D$10</f>
-        <v>IodoYRS Amber+ Clone 2 IodoY- Replicate 3</v>
+        <f>Setup!$G$5</f>
+        <v>IodoYRS Amber+ Clone 3 IodoY+ Replicate 1</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="str">
-        <f>Setup!$G$5</f>
-        <v>IodoYRS Amber+ Clone 3 IodoY+ Replicate 1</v>
+        <f>Setup!$G$6</f>
+        <v>IodoYRS Amber+ Clone 3 IodoY+ Replicate 2</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="str">
-        <f>Setup!$G$6</f>
-        <v>IodoYRS Amber+ Clone 3 IodoY+ Replicate 2</v>
+        <f>Setup!$G$7</f>
+        <v>IodoYRS Amber+ Clone 3 IodoY+ Replicate 3</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="str">
-        <f>Setup!$G$7</f>
-        <v>IodoYRS Amber+ Clone 3 IodoY+ Replicate 3</v>
+        <f>Setup!$G$8</f>
+        <v>IodoYRS Amber+ Clone 3 IodoY- Replicate 1</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="str">
-        <f>Setup!$G$8</f>
-        <v>IodoYRS Amber+ Clone 3 IodoY- Replicate 1</v>
+        <f>Setup!$G$9</f>
+        <v>IodoYRS Amber+ Clone 3 IodoY- Replicate 2</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="str">
-        <f>Setup!$G$9</f>
-        <v>IodoYRS Amber+ Clone 3 IodoY- Replicate 2</v>
+        <f>Setup!$G$10</f>
+        <v>IodoYRS Amber+ Clone 3 IodoY- Replicate 3</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="str">
-        <f>Setup!$G$10</f>
-        <v>IodoYRS Amber+ Clone 3 IodoY- Replicate 3</v>
+        <f>Setup!$A$13</f>
+        <v>IodoYRS Amber- Clone 1 IodoY+ Replicate 1</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="str">
-        <f>Setup!$A$13</f>
-        <v>IodoYRS Amber- Clone 1 IodoY+ Replicate 1</v>
+        <f>Setup!$A$14</f>
+        <v>IodoYRS Amber- Clone 1 IodoY+ Replicate 2</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="str">
-        <f>Setup!$A$14</f>
-        <v>IodoYRS Amber- Clone 1 IodoY+ Replicate 2</v>
+        <f>Setup!$A$15</f>
+        <v>IodoYRS Amber- Clone 1 IodoY+ Replicate 3</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="str">
-        <f>Setup!$A$15</f>
-        <v>IodoYRS Amber- Clone 1 IodoY+ Replicate 3</v>
+        <f>Setup!$A$16</f>
+        <v>IodoYRS Amber- Clone 1 IodoY- Replicate 1</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="str">
-        <f>Setup!$A$16</f>
-        <v>IodoYRS Amber- Clone 1 IodoY- Replicate 1</v>
+        <f>Setup!$A$17</f>
+        <v>IodoYRS Amber- Clone 1 IodoY- Replicate 2</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="str">
-        <f>Setup!$A$17</f>
-        <v>IodoYRS Amber- Clone 1 IodoY- Replicate 2</v>
+        <f>Setup!$A$18</f>
+        <v>IodoYRS Amber- Clone 1 IodoY- Replicate 3</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="str">
-        <f>Setup!$A$18</f>
-        <v>IodoYRS Amber- Clone 1 IodoY- Replicate 3</v>
+        <f>Setup!$D$13</f>
+        <v>IodoYRS Amber- Clone 2 IodoY+ Replicate 1</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="str">
-        <f>Setup!$D$13</f>
-        <v>IodoYRS Amber- Clone 2 IodoY+ Replicate 1</v>
+        <f>Setup!$D$14</f>
+        <v>IodoYRS Amber- Clone 2 IodoY+ Replicate 2</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="str">
-        <f>Setup!$D$14</f>
-        <v>IodoYRS Amber- Clone 2 IodoY+ Replicate 2</v>
+        <f>Setup!$D$15</f>
+        <v>IodoYRS Amber- Clone 2 IodoY+ Replicate 3</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="str">
-        <f>Setup!$D$15</f>
-        <v>IodoYRS Amber- Clone 2 IodoY+ Replicate 3</v>
+        <f>Setup!$D$16</f>
+        <v>IodoYRS Amber- Clone 2 IodoY- Replicate 1</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="str">
-        <f>Setup!$D$16</f>
-        <v>IodoYRS Amber- Clone 2 IodoY- Replicate 1</v>
+        <f>Setup!$D$17</f>
+        <v>IodoYRS Amber- Clone 2 IodoY- Replicate 2</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="str">
-        <f>Setup!$D$17</f>
-        <v>IodoYRS Amber- Clone 2 IodoY- Replicate 2</v>
+        <f>Setup!$D$18</f>
+        <v>IodoYRS Amber- Clone 2 IodoY- Replicate 3</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="str">
-        <f>Setup!$D$18</f>
-        <v>IodoYRS Amber- Clone 2 IodoY- Replicate 3</v>
+        <f>Setup!$G$13</f>
+        <v>IodoYRS Amber- Clone 3 IodoY+ Replicate 1</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="str">
-        <f>Setup!$G$13</f>
-        <v>IodoYRS Amber- Clone 3 IodoY+ Replicate 1</v>
+        <f>Setup!$G$14</f>
+        <v>IodoYRS Amber- Clone 3 IodoY+ Replicate 2</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="str">
-        <f>Setup!$G$14</f>
-        <v>IodoYRS Amber- Clone 3 IodoY+ Replicate 2</v>
+        <f>Setup!$G$15</f>
+        <v>IodoYRS Amber- Clone 3 IodoY+ Replicate 3</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="str">
-        <f>Setup!$G$15</f>
-        <v>IodoYRS Amber- Clone 3 IodoY+ Replicate 3</v>
+        <f>Setup!$G$16</f>
+        <v>IodoYRS Amber- Clone 3 IodoY- Replicate 1</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="str">
-        <f>Setup!$G$16</f>
-        <v>IodoYRS Amber- Clone 3 IodoY- Replicate 1</v>
+        <f>Setup!$G$17</f>
+        <v>IodoYRS Amber- Clone 3 IodoY- Replicate 2</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="str">
-        <f>Setup!$G$17</f>
-        <v>IodoYRS Amber- Clone 3 IodoY- Replicate 2</v>
+        <f>Setup!$G$18</f>
+        <v>IodoYRS Amber- Clone 3 IodoY- Replicate 3</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="str">
-        <f>Setup!$G$18</f>
-        <v>IodoYRS Amber- Clone 3 IodoY- Replicate 3</v>
+        <f>Setup!$A$21</f>
+        <v>AminoYRS Amber+ Clone 1 AminoY+ Replicate 1</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="str">
-        <f>Setup!$A$21</f>
-        <v>AminoYRS Amber+ Clone 1 AminoY+ Replicate 1</v>
+        <f>Setup!$A$22</f>
+        <v>AminoYRS Amber+ Clone 1 AminoY+ Replicate 2</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="str">
-        <f>Setup!$A$22</f>
-        <v>AminoYRS Amber+ Clone 1 AminoY+ Replicate 2</v>
+        <f>Setup!$A$23</f>
+        <v>AminoYRS Amber+ Clone 1 AminoY+ Replicate 3</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="str">
-        <f>Setup!$A$23</f>
-        <v>AminoYRS Amber+ Clone 1 AminoY+ Replicate 3</v>
+        <f>Setup!$A$24</f>
+        <v>AminoYRS Amber+ Clone 1 AminoY- Replicate 1</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="str">
-        <f>Setup!$A$24</f>
-        <v>AminoYRS Amber+ Clone 1 AminoY- Replicate 1</v>
+        <f>Setup!$A$25</f>
+        <v>AminoYRS Amber+ Clone 1 AminoY- Replicate 2</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="str">
-        <f>Setup!$A$25</f>
-        <v>AminoYRS Amber+ Clone 1 AminoY- Replicate 2</v>
+        <f>Setup!$A$26</f>
+        <v>AminoYRS Amber+ Clone 1 AminoY- Replicate 3</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="str">
-        <f>Setup!$A$26</f>
-        <v>AminoYRS Amber+ Clone 1 AminoY- Replicate 3</v>
+        <f>Setup!$D$21</f>
+        <v>AminoYRS Amber+ Clone 2 AminoY+ Replicate 1</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="str">
-        <f>Setup!$D$21</f>
-        <v>AminoYRS Amber+ Clone 2 AminoY+ Replicate 1</v>
+        <f>Setup!$D$22</f>
+        <v>AminoYRS Amber+ Clone 2 AminoY+ Replicate 2</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="str">
-        <f>Setup!$D$22</f>
-        <v>AminoYRS Amber+ Clone 2 AminoY+ Replicate 2</v>
+        <f>Setup!$D$23</f>
+        <v>AminoYRS Amber+ Clone 2 AminoY+ Replicate 3</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="str">
-        <f>Setup!$D$23</f>
-        <v>AminoYRS Amber+ Clone 2 AminoY+ Replicate 3</v>
+        <f>Setup!$D$24</f>
+        <v>AminoYRS Amber+ Clone 2 AminoY- Replicate 1</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="str">
-        <f>Setup!$D$24</f>
-        <v>AminoYRS Amber+ Clone 2 AminoY- Replicate 1</v>
+        <f>Setup!$D$25</f>
+        <v>AminoYRS Amber+ Clone 2 AminoY- Replicate 2</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="str">
-        <f>Setup!$D$25</f>
-        <v>AminoYRS Amber+ Clone 2 AminoY- Replicate 2</v>
+        <f>Setup!$D$26</f>
+        <v>AminoYRS Amber+ Clone 2 AminoY- Replicate 3</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="str">
-        <f>Setup!$D$26</f>
-        <v>AminoYRS Amber+ Clone 2 AminoY- Replicate 3</v>
+        <f>Setup!$G$21</f>
+        <v>AminoYRS Amber+ Clone 3 AminoY+ Replicate 1</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="str">
-        <f>Setup!$G$21</f>
-        <v>AminoYRS Amber+ Clone 3 AminoY+ Replicate 1</v>
+        <f>Setup!$G$22</f>
+        <v>AminoYRS Amber+ Clone 3 AminoY+ Replicate 2</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="str">
-        <f>Setup!$G$22</f>
-        <v>AminoYRS Amber+ Clone 3 AminoY+ Replicate 2</v>
+        <f>Setup!$G$23</f>
+        <v>AminoYRS Amber+ Clone 3 AminoY+ Replicate 3</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="str">
-        <f>Setup!$G$23</f>
-        <v>AminoYRS Amber+ Clone 3 AminoY+ Replicate 3</v>
+        <f>Setup!$G$24</f>
+        <v>AminoYRS Amber+ Clone 3 AminoY- Replicate 1</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="str">
-        <f>Setup!$G$24</f>
-        <v>AminoYRS Amber+ Clone 3 AminoY- Replicate 1</v>
+        <f>Setup!$G$25</f>
+        <v>AminoYRS Amber+ Clone 3 AminoY- Replicate 2</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="str">
-        <f>Setup!$G$25</f>
-        <v>AminoYRS Amber+ Clone 3 AminoY- Replicate 2</v>
+        <f>Setup!$G$26</f>
+        <v>AminoYRS Amber+ Clone 3 AminoY- Replicate 3</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="str">
-        <f>Setup!$G$26</f>
-        <v>AminoYRS Amber+ Clone 3 AminoY- Replicate 3</v>
+        <f>Setup!$A$29</f>
+        <v>AminoYRS Amber- Clone 1 AminoY+ Replicate 1</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="str">
-        <f>Setup!$A$29</f>
-        <v>AminoYRS Amber- Clone 1 AminoY+ Replicate 1</v>
+        <f>Setup!$A$30</f>
+        <v>AminoYRS Amber- Clone 1 AminoY+ Replicate 2</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="str">
-        <f>Setup!$A$30</f>
-        <v>AminoYRS Amber- Clone 1 AminoY+ Replicate 2</v>
+        <f>Setup!$A$31</f>
+        <v>AminoYRS Amber- Clone 1 AminoY+ Replicate 3</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="str">
-        <f>Setup!$A$31</f>
-        <v>AminoYRS Amber- Clone 1 AminoY+ Replicate 3</v>
+        <f>Setup!$A$32</f>
+        <v>AminoYRS Amber- Clone 1 AminoY- Replicate 1</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="str">
-        <f>Setup!$A$32</f>
-        <v>AminoYRS Amber- Clone 1 AminoY- Replicate 1</v>
+        <f>Setup!$A$33</f>
+        <v>AminoYRS Amber- Clone 1 AminoY- Replicate 2</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="str">
-        <f>Setup!$A$33</f>
-        <v>AminoYRS Amber- Clone 1 AminoY- Replicate 2</v>
+        <f>Setup!$A$34</f>
+        <v>AminoYRS Amber- Clone 1 AminoY- Replicate 3</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="str">
-        <f>Setup!$A$34</f>
-        <v>AminoYRS Amber- Clone 1 AminoY- Replicate 3</v>
+        <f>Setup!$D$29</f>
+        <v>AminoYRS Amber- Clone 2 AminoY+ Replicate 1</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="str">
-        <f>Setup!$D$29</f>
-        <v>AminoYRS Amber- Clone 2 AminoY+ Replicate 1</v>
+        <f>Setup!$D$30</f>
+        <v>AminoYRS Amber- Clone 2 AminoY+ Replicate 2</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="str">
-        <f>Setup!$D$30</f>
-        <v>AminoYRS Amber- Clone 2 AminoY+ Replicate 2</v>
+        <f>Setup!$D$31</f>
+        <v>AminoYRS Amber- Clone 2 AminoY+ Replicate 3</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="str">
-        <f>Setup!$D$31</f>
-        <v>AminoYRS Amber- Clone 2 AminoY+ Replicate 3</v>
+        <f>Setup!$D$32</f>
+        <v>AminoYRS Amber- Clone 2 AminoY- Replicate 1</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="str">
-        <f>Setup!$D$32</f>
-        <v>AminoYRS Amber- Clone 2 AminoY- Replicate 1</v>
+        <f>Setup!$D$33</f>
+        <v>AminoYRS Amber- Clone 2 AminoY- Replicate 2</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="str">
-        <f>Setup!$D$33</f>
-        <v>AminoYRS Amber- Clone 2 AminoY- Replicate 2</v>
+        <f>Setup!$D$34</f>
+        <v>AminoYRS Amber- Clone 2 AminoY- Replicate 3</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="str">
-        <f>Setup!$D$34</f>
-        <v>AminoYRS Amber- Clone 2 AminoY- Replicate 3</v>
+        <f>Setup!$G$29</f>
+        <v>AminoYRS Amber- Clone 3 AminoY+ Replicate 1</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="str">
-        <f>Setup!$G$29</f>
-        <v>AminoYRS Amber- Clone 3 AminoY+ Replicate 1</v>
+        <f>Setup!$G$30</f>
+        <v>AminoYRS Amber- Clone 3 AminoY+ Replicate 2</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="str">
-        <f>Setup!$G$30</f>
-        <v>AminoYRS Amber- Clone 3 AminoY+ Replicate 2</v>
+        <f>Setup!$G$31</f>
+        <v>AminoYRS Amber- Clone 3 AminoY+ Replicate 3</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="str">
-        <f>Setup!$G$31</f>
-        <v>AminoYRS Amber- Clone 3 AminoY+ Replicate 3</v>
+        <f>Setup!$G$32</f>
+        <v>AminoYRS Amber- Clone 3 AminoY- Replicate 1</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="str">
-        <f>Setup!$G$32</f>
-        <v>AminoYRS Amber- Clone 3 AminoY- Replicate 1</v>
+        <f>Setup!$G$33</f>
+        <v>AminoYRS Amber- Clone 3 AminoY- Replicate 2</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="str">
-        <f>Setup!$G$33</f>
-        <v>AminoYRS Amber- Clone 3 AminoY- Replicate 2</v>
+        <f>Setup!$G$34</f>
+        <v>AminoYRS Amber- Clone 3 AminoY- Replicate 3</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="str">
-        <f>Setup!$G$34</f>
-        <v>AminoYRS Amber- Clone 3 AminoY- Replicate 3</v>
+        <f>Setup!$A$37</f>
+        <v>LB IodoY+ Replicate 1</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="str">
-        <f>Setup!$A$37</f>
-        <v>LB IodoY+ Replicate 1</v>
+        <f>Setup!$A$38</f>
+        <v>LB IodoY+ Replicate 2</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="str">
-        <f>Setup!$A$38</f>
-        <v>LB IodoY+ Replicate 2</v>
+        <f>Setup!$A$39</f>
+        <v>LB IodoY+ Replicate 3</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="str">
-        <f>Setup!$A$39</f>
-        <v>LB IodoY+ Replicate 3</v>
+        <f>Setup!$A$42</f>
+        <v>LB AminoY+ Replicate 1</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="str">
-        <f>Setup!$A$42</f>
-        <v>LB AminoY+ Replicate 1</v>
+        <f>Setup!$A$43</f>
+        <v>LB AminoY+ Replicate 2</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="str">
-        <f>Setup!$A$43</f>
-        <v>LB AminoY+ Replicate 2</v>
+        <f>Setup!$A$44</f>
+        <v>LB AminoY+ Replicate 3</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="str">
-        <f>Setup!$A$44</f>
-        <v>LB AminoY+ Replicate 3</v>
+        <f>Setup!$A$47</f>
+        <v>LB Water+ Replicate 1</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="str">
-        <f>Setup!$A$47</f>
-        <v>LB Water+ Replicate 1</v>
+        <f>Setup!$A$48</f>
+        <v>LB Water+ Replicate 2</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="str">
-        <f>Setup!$A$48</f>
-        <v>LB Water+ Replicate 2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" t="str">
         <f>Setup!$A$49</f>
         <v>LB Water+ Replicate 3</v>
       </c>

</xml_diff>